<commit_message>
updated dbo_species and reviewed helcom handler
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_sedtype.xlsx
+++ b/nbs/files/lut/dbo_sedtype.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621B13CF-C4D9-E041-B09C-5572580B156E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB48AE4-88D8-634F-858A-27F670D2946E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="500" windowWidth="23900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -844,7 +844,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1617,21 +1617,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C266C02A97D1D41B60FC5BB4AB3B561" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="627c5da731661f4bf76604184727f2d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3c01d95-e195-4940-9fb4-afa395d98e0b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bf665a11c7ceb3b31f5a9dbdfc3fcda" ns2:_="">
     <xsd:import namespace="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
@@ -1763,24 +1748,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{204CBD9F-684A-445C-A7C1-94CB78F0C545}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A455860D-547D-49FF-8782-6C38DF3CF22F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEEC0707-DFF7-4054-9B24-5AA1806D32FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1796,4 +1779,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A455860D-547D-49FF-8782-6C38DF3CF22F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{204CBD9F-684A-445C-A7C1-94CB78F0C545}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>